<commit_message>
Removed some resources and read dynamic threshold params from config
</commit_message>
<xml_diff>
--- a/DynamicThresholdComparison.xlsx
+++ b/DynamicThresholdComparison.xlsx
@@ -24,36 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">null   10%   20%   30%   40%   50%   60%   70%   80%   90%   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,1   0,09   0,18   0,27   0,36   0,45   0,54   0,63   0,72   0,81   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,2   0,08   0,16   0,24   0,32   0,40   0,48   0,56   0,64   0,72   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,3   0,07   0,14   0,21   0,28   0,35   0,42   0,49   0,56   0,63   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,4   0,06   0,12   0,18   0,24   0,30   0,36   0,42   0,48   0,54   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,5   0,05   0,10   0,15   0,20   0,25   0,30   0,35   0,40   0,45   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,6   0,04   0,08   0,12   0,16   0,20   0,24   0,28   0,32   0,36   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,7   0,03   0,06   0,09   0,12   0,15   0,18   0,21   0,24   0,27   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,8   0,02   0,04   0,06   0,08   0,10   0,12   0,14   0,16   0,18   </t>
-  </si>
-  <si>
-    <t>0,9   0,01   0,02   0,03   0,04   0,05   0,06   0,07   0,08   0,09</t>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -90,8 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,62 +346,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="B1" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>0.01</v>
+      </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+      <c r="D2">
+        <v>0.09</v>
+      </c>
+      <c r="E2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.18</v>
+      </c>
+      <c r="G2">
+        <v>0.23</v>
+      </c>
+      <c r="H2">
+        <v>0.27</v>
+      </c>
+      <c r="I2">
+        <v>0.36</v>
+      </c>
+      <c r="J2">
+        <v>0.45</v>
+      </c>
+      <c r="K2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>0.01</v>
+      </c>
+      <c r="C3">
+        <v>0.04</v>
+      </c>
+      <c r="D3">
+        <v>0.08</v>
+      </c>
+      <c r="E3">
+        <v>0.12</v>
+      </c>
+      <c r="F3">
+        <v>0.16</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3">
+        <v>0.24</v>
+      </c>
+      <c r="I3">
+        <v>0.32</v>
+      </c>
+      <c r="J3">
+        <v>0.4</v>
+      </c>
+      <c r="K3">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>0.01</v>
+      </c>
+      <c r="C4">
+        <v>0.03</v>
+      </c>
+      <c r="D4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.17</v>
+      </c>
+      <c r="H4">
+        <v>0.21</v>
+      </c>
+      <c r="I4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J4">
+        <v>0.35</v>
+      </c>
+      <c r="K4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <v>0.03</v>
+      </c>
+      <c r="D5">
+        <v>0.06</v>
+      </c>
+      <c r="E5">
+        <v>0.09</v>
+      </c>
+      <c r="F5">
+        <v>0.12</v>
+      </c>
+      <c r="G5">
+        <v>0.15</v>
+      </c>
+      <c r="H5">
+        <v>0.18</v>
+      </c>
+      <c r="I5">
+        <v>0.24</v>
+      </c>
+      <c r="J5">
+        <v>0.3</v>
+      </c>
+      <c r="K5">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
+        <v>0.03</v>
+      </c>
+      <c r="D6">
+        <v>0.05</v>
+      </c>
+      <c r="E6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>0.12</v>
+      </c>
+      <c r="H6">
+        <v>0.15</v>
+      </c>
+      <c r="I6">
+        <v>0.2</v>
+      </c>
+      <c r="J6">
+        <v>0.25</v>
+      </c>
+      <c r="K6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.02</v>
+      </c>
+      <c r="D7">
+        <v>0.04</v>
+      </c>
+      <c r="E7">
+        <v>0.06</v>
+      </c>
+      <c r="F7">
+        <v>0.08</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.12</v>
+      </c>
+      <c r="I7">
+        <v>0.16</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8">
+        <v>0.03</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>0.06</v>
+      </c>
+      <c r="G8">
+        <v>0.08</v>
+      </c>
+      <c r="H8">
+        <v>0.09</v>
+      </c>
+      <c r="I8">
+        <v>0.12</v>
+      </c>
+      <c r="J8">
+        <v>0.15</v>
+      </c>
+      <c r="K8">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.02</v>
+      </c>
+      <c r="E9">
+        <v>0.03</v>
+      </c>
+      <c r="F9">
+        <v>0.04</v>
+      </c>
+      <c r="G9">
+        <v>0.05</v>
+      </c>
+      <c r="H9">
+        <v>0.06</v>
+      </c>
+      <c r="I9">
+        <v>0.08</v>
+      </c>
+      <c r="J9">
+        <v>0.1</v>
+      </c>
+      <c r="K9">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+      <c r="D10">
+        <v>0.01</v>
+      </c>
+      <c r="E10">
+        <v>0.02</v>
+      </c>
+      <c r="F10">
+        <v>0.02</v>
+      </c>
+      <c r="G10">
+        <v>0.03</v>
+      </c>
+      <c r="H10">
+        <v>0.03</v>
+      </c>
+      <c r="I10">
+        <v>0.04</v>
+      </c>
+      <c r="J10">
+        <v>0.05</v>
+      </c>
+      <c r="K10">
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>